<commit_message>
adding datasheet and component
</commit_message>
<xml_diff>
--- a/resources/component_list.xlsx
+++ b/resources/component_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srtls\Documents\GitHub\Capstone_Duayenler\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2DBC59-5641-4C1E-8A85-8F96B1462765}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43CBD58-B06E-4EE6-B09D-34673FB99F8D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>Component Name</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>waveshare Lase sensor</t>
-  </si>
-  <si>
     <t>82.16TL</t>
   </si>
   <si>
@@ -135,6 +132,51 @@
   </si>
   <si>
     <t>Digital o/p, laser based distance sensor for 0.8-1.5m</t>
+  </si>
+  <si>
+    <t>Reflective Optical Sensor with Transistor Output</t>
+  </si>
+  <si>
+    <t>.99TL</t>
+  </si>
+  <si>
+    <t>kalsörde</t>
+  </si>
+  <si>
+    <t>https://www.robotistan.com/tcrt5000-kizilotesi-sensor?query=k%C4%B1z%C4%B1l%C3%B6tesi%20sens%C3%B6r&amp;</t>
+  </si>
+  <si>
+    <t>IR sensör for 0.2 to 15mm</t>
+  </si>
+  <si>
+    <t>IR sensor card (8)</t>
+  </si>
+  <si>
+    <t>67TL</t>
+  </si>
+  <si>
+    <t>https://www.robotistan.com/qtr-8rc-kizilotesi-sensor?query=k%C4%B1z%C4%B1l%C3%B6tesi%20sens%C3%B6r&amp;</t>
+  </si>
+  <si>
+    <t>IR sensör for 3mm</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>waveshare Laser sensor</t>
+  </si>
+  <si>
+    <t>TF mini LiDAR</t>
+  </si>
+  <si>
+    <t>273.83TL</t>
+  </si>
+  <si>
+    <t>https://www.direnc.net/tf-mini-lidar-tof-lazer-menzil-sensoru-dfrobot</t>
+  </si>
+  <si>
+    <t>Laser menzil sensörü for mapping</t>
   </si>
 </sst>
 </file>
@@ -527,7 +569,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -711,43 +753,75 @@
     </row>
     <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="2" t="s">
+    </row>
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:16" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
@@ -823,9 +897,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" xr:uid="{CF819F7D-5CA9-4288-A0CF-1B8A670E1C19}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{EC06E0A4-B437-4578-A0F3-91EDF1CD2028}"/>
+    <hyperlink ref="E9" r:id="rId3" xr:uid="{F209609A-F13D-4A57-A341-851EE1B89B61}"/>
+    <hyperlink ref="E10" r:id="rId4" xr:uid="{350154C3-1F64-44DE-8B7D-51518698B62C}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
linked in excel turned clickable
</commit_message>
<xml_diff>
--- a/resources/component_list.xlsx
+++ b/resources/component_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srtls\Documents\GitHub\Capstone_Duayenler\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Halil Temurtaş\Desktop\Ekstra\Capstone_Duayenler\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF05110D-61A7-4C75-87BF-640EDED24F81}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6237F8F-E87A-4792-8D71-480DD21D4A7B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,7 +265,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Köprü" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -636,7 +636,7 @@
       <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -666,7 +666,7 @@
       <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -696,7 +696,7 @@
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -726,7 +726,7 @@
       <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -756,7 +756,7 @@
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -923,9 +923,14 @@
     <hyperlink ref="E9" r:id="rId3" xr:uid="{F209609A-F13D-4A57-A341-851EE1B89B61}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{350154C3-1F64-44DE-8B7D-51518698B62C}"/>
     <hyperlink ref="E11" r:id="rId5" xr:uid="{D2ACA959-33F8-4E2E-97B8-CBDA6770CAEC}"/>
+    <hyperlink ref="E2" r:id="rId6" xr:uid="{BE3DD6A4-ACFF-4BCF-9660-4F673994E7C3}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{7A58C143-2A99-4A56-B2A8-4A5CA43E1E70}"/>
+    <hyperlink ref="E4" r:id="rId8" xr:uid="{2084FC83-6DF1-4176-BA82-A9ACFAF716A5}"/>
+    <hyperlink ref="E5" r:id="rId9" xr:uid="{00F155BF-0893-4EC1-9FAC-8515DA39C176}"/>
+    <hyperlink ref="E6" r:id="rId10" xr:uid="{44F1059C-3448-4BC5-B54A-EDC131C39729}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId11"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
datasheet + componenet added
</commit_message>
<xml_diff>
--- a/resources/component_list.xlsx
+++ b/resources/component_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srtls\Documents\GitHub\Capstone_Duayenler\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C308D3BE-3116-41A1-BC76-4B16BC913DC9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F557D7FB-00A5-45A7-B224-10A41E06F0A2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
   <si>
     <t>Component Name</t>
   </si>
@@ -272,6 +272,18 @@
   </si>
   <si>
     <t>micro motor mid current (0.8A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ultrasonic distance sensor </t>
+  </si>
+  <si>
+    <t>8 TL</t>
+  </si>
+  <si>
+    <t>https://www.robotistan.com/hc-sr04-ultrasonik-mesafe-sensoru?_sgm_campaign=scn_6186b7884aa16000&amp;_sgm_source=1751&amp;_sgm_action=click</t>
+  </si>
+  <si>
+    <t>40KHz sonic measurement 2cm to 4m 3mm precision</t>
   </si>
 </sst>
 </file>
@@ -747,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1117,17 +1129,31 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="F18" s="2" t="s">
+      <c r="A18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="F31" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="F19" s="2" t="s">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="F32" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="F20" s="2" t="s">
+    <row r="33" spans="6:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="F33" s="2" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1154,6 +1180,7 @@
     <hyperlink ref="E15" r:id="rId19" xr:uid="{0CE1CE8E-209D-4BD1-9507-BD7BDFB283C1}"/>
     <hyperlink ref="E16" r:id="rId20" xr:uid="{E8C1CE80-064C-424F-90D1-4A6A27C0FD30}"/>
     <hyperlink ref="E17" r:id="rId21" xr:uid="{9AEB2D66-67B5-4471-8400-FEAAE0D3C14F}"/>
+    <hyperlink ref="E18" r:id="rId22" xr:uid="{6A643E2A-B345-4C79-840C-5E414534A084}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>